<commit_message>
Missing km for last oil change.
</commit_message>
<xml_diff>
--- a/book-keeping.xlsx
+++ b/book-keeping.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Car!$A$1:$K$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Car!$A$1:$K$101</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -154,19 +154,27 @@
   </si>
   <si>
     <t>ETR (Markham Festivals)</t>
+  </si>
+  <si>
+    <t>Transfer from "My Savings"</t>
+  </si>
+  <si>
+    <t>Oil Change</t>
+  </si>
+  <si>
+    <t>Minimum Balance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +198,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -387,12 +403,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -401,21 +417,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,15 +441,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,8 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -753,12 +770,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M230"/>
+  <dimension ref="A1:P226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="855" topLeftCell="A38" activePane="bottomLeft"/>
-      <selection activeCell="L1" sqref="A1:XFD2"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72:K72"/>
+      <pane ySplit="900" topLeftCell="A52" activePane="bottomLeft"/>
+      <selection activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,35 +793,42 @@
     <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="32">
+        <v>222.42</v>
+      </c>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="35"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -823,12 +847,25 @@
       <c r="G2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="32">
+        <v>82.97</v>
+      </c>
+      <c r="O2" s="33">
+        <f>N2+N1</f>
+        <v>305.39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>42856</v>
       </c>
@@ -855,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>42875</v>
       </c>
@@ -884,7 +921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>42877</v>
       </c>
@@ -911,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>42878</v>
       </c>
@@ -942,7 +979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>42879</v>
       </c>
@@ -969,7 +1006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>42881</v>
       </c>
@@ -996,7 +1033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>42870</v>
       </c>
@@ -1021,7 +1058,7 @@
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>42882</v>
       </c>
@@ -1044,7 +1081,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>42882</v>
       </c>
@@ -1069,7 +1106,7 @@
       </c>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>42884</v>
       </c>
@@ -1096,7 +1133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>42884</v>
       </c>
@@ -1123,7 +1160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42886</v>
       </c>
@@ -1152,7 +1189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>42886</v>
       </c>
@@ -1181,7 +1218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>42887</v>
       </c>
@@ -2514,7 +2551,7 @@
       </c>
       <c r="K64" s="22"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>42947</v>
       </c>
@@ -2539,7 +2576,7 @@
       </c>
       <c r="K65" s="22"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>42953</v>
       </c>
@@ -2570,7 +2607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>42955</v>
       </c>
@@ -2595,374 +2632,467 @@
       </c>
       <c r="K67" s="23"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>42956</v>
       </c>
       <c r="B68" s="9"/>
-      <c r="C68" s="15">
-        <v>355.93</v>
-      </c>
+      <c r="C68" s="15"/>
       <c r="D68" s="19">
         <f>IF(NOT(ISBLANK($A68)),SUM(B$3:B68)-SUM(C$3:C68),"")</f>
-        <v>262.15999999999985</v>
+        <v>618.08999999999969</v>
       </c>
       <c r="E68" s="9"/>
-      <c r="F68" s="15"/>
+      <c r="F68" s="15">
+        <v>33</v>
+      </c>
       <c r="G68" s="19">
         <f>IF(NOT(ISBLANK($A68)),SUM(E$3:E68)-SUM(F$3:F68),"")</f>
-        <v>-809.24000000000024</v>
+        <v>-842.24000000000024</v>
       </c>
       <c r="H68" s="10" t="b">
         <v>1</v>
       </c>
       <c r="I68" s="21"/>
       <c r="J68" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K68" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
-        <v>42956</v>
-      </c>
-      <c r="B69" s="7">
-        <v>400</v>
-      </c>
-      <c r="C69" s="14"/>
+        <v>42957</v>
+      </c>
+      <c r="B69" s="7"/>
+      <c r="C69" s="14">
+        <v>355.93</v>
+      </c>
       <c r="D69" s="18">
         <f>IF(NOT(ISBLANK($A69)),SUM(B$3:B69)-SUM(C$3:C69),"")</f>
-        <v>662.15999999999985</v>
+        <v>262.15999999999985</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="14"/>
       <c r="G69" s="18">
         <f>IF(NOT(ISBLANK($A69)),SUM(E$3:E69)-SUM(F$3:F69),"")</f>
-        <v>-809.24000000000024</v>
-      </c>
-      <c r="H69" s="8"/>
+        <v>-842.24000000000024</v>
+      </c>
+      <c r="H69" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I69" s="20"/>
       <c r="J69" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K69" s="22"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="K69" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>42957</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="14">
-        <v>5</v>
+        <v>351.77</v>
       </c>
       <c r="D70" s="18">
         <f>IF(NOT(ISBLANK($A70)),SUM(B$3:B70)-SUM(C$3:C70),"")</f>
-        <v>657.15999999999985</v>
-      </c>
-      <c r="E70" s="7"/>
+        <v>-89.610000000000582</v>
+      </c>
+      <c r="E70" s="7">
+        <v>351.77</v>
+      </c>
       <c r="F70" s="14"/>
       <c r="G70" s="18">
         <f>IF(NOT(ISBLANK($A70)),SUM(E$3:E70)-SUM(F$3:F70),"")</f>
-        <v>-809.24000000000024</v>
-      </c>
-      <c r="H70" s="8" t="b">
-        <v>1</v>
-      </c>
+        <v>-490.47000000000025</v>
+      </c>
+      <c r="H70" s="8"/>
       <c r="I70" s="20"/>
       <c r="J70" s="8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="K70" s="22"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
-        <v>42956</v>
-      </c>
-      <c r="B71" s="7"/>
+        <v>42957</v>
+      </c>
+      <c r="B71" s="7">
+        <v>400</v>
+      </c>
       <c r="C71" s="14"/>
       <c r="D71" s="18">
         <f>IF(NOT(ISBLANK($A71)),SUM(B$3:B71)-SUM(C$3:C71),"")</f>
-        <v>657.15999999999985</v>
+        <v>310.38999999999942</v>
       </c>
       <c r="E71" s="7"/>
-      <c r="F71" s="14">
-        <v>33</v>
-      </c>
+      <c r="F71" s="14"/>
       <c r="G71" s="18">
         <f>IF(NOT(ISBLANK($A71)),SUM(E$3:E71)-SUM(F$3:F71),"")</f>
-        <v>-842.24000000000024</v>
-      </c>
-      <c r="H71" s="8" t="b">
-        <v>1</v>
-      </c>
+        <v>-490.47000000000025</v>
+      </c>
+      <c r="H71" s="8"/>
       <c r="I71" s="20"/>
       <c r="J71" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K71" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="K71" s="22"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
-        <v>42956</v>
+        <v>42957</v>
       </c>
       <c r="B72" s="9"/>
       <c r="C72" s="15">
-        <v>351.77</v>
+        <v>5</v>
       </c>
       <c r="D72" s="19">
         <f>IF(NOT(ISBLANK($A72)),SUM(B$3:B72)-SUM(C$3:C72),"")</f>
         <v>305.38999999999942</v>
       </c>
-      <c r="E72" s="9">
-        <v>351.77</v>
-      </c>
+      <c r="E72" s="9"/>
       <c r="F72" s="15"/>
       <c r="G72" s="19">
         <f>IF(NOT(ISBLANK($A72)),SUM(E$3:E72)-SUM(F$3:F72),"")</f>
         <v>-490.47000000000025</v>
       </c>
-      <c r="H72" s="10"/>
+      <c r="H72" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I72" s="21"/>
       <c r="J72" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K72" s="23"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="K72" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="12">
+        <v>42957</v>
+      </c>
       <c r="B73" s="9"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="19" t="str">
+      <c r="C73" s="15">
+        <v>222.42</v>
+      </c>
+      <c r="D73" s="19">
         <f>IF(NOT(ISBLANK($A73)),SUM(B$3:B73)-SUM(C$3:C73),"")</f>
-        <v/>
+        <v>82.969999999999345</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="15"/>
-      <c r="G73" s="19" t="str">
+      <c r="G73" s="19">
         <f>IF(NOT(ISBLANK($A73)),SUM(E$3:E73)-SUM(F$3:F73),"")</f>
-        <v/>
+        <v>-490.47000000000025</v>
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="21"/>
-      <c r="J73" s="10"/>
+      <c r="J73" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="K73" s="23"/>
-      <c r="M73" s="37"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="12">
+        <v>42958</v>
+      </c>
       <c r="B74" s="9"/>
       <c r="C74" s="15"/>
-      <c r="D74" s="19" t="str">
+      <c r="D74" s="19">
         <f>IF(NOT(ISBLANK($A74)),SUM(B$3:B74)-SUM(C$3:C74),"")</f>
-        <v/>
+        <v>82.969999999999345</v>
       </c>
       <c r="E74" s="9"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="19" t="str">
+      <c r="F74" s="15">
+        <v>187.58</v>
+      </c>
+      <c r="G74" s="19">
         <f>IF(NOT(ISBLANK($A74)),SUM(E$3:E74)-SUM(F$3:F74),"")</f>
-        <v/>
-      </c>
-      <c r="H74" s="10"/>
+        <v>-678.05000000000018</v>
+      </c>
+      <c r="H74" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I74" s="21"/>
-      <c r="J74" s="10"/>
+      <c r="J74" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="K74" s="23"/>
-      <c r="M74" s="37"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="18" t="str">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="12">
+        <v>42962</v>
+      </c>
+      <c r="B75" s="9">
+        <v>450</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="19">
         <f>IF(NOT(ISBLANK($A75)),SUM(B$3:B75)-SUM(C$3:C75),"")</f>
-        <v/>
-      </c>
-      <c r="E75" s="7"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="18" t="str">
+        <v>532.96999999999935</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="19">
         <f>IF(NOT(ISBLANK($A75)),SUM(E$3:E75)-SUM(F$3:F75),"")</f>
-        <v/>
-      </c>
-      <c r="H75" s="8"/>
-      <c r="I75" s="20"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="22"/>
-      <c r="M75" s="38"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+        <v>-678.05000000000018</v>
+      </c>
+      <c r="H75" s="10"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K75" s="23"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="11">
+        <v>42963</v>
+      </c>
       <c r="B76" s="7"/>
       <c r="C76" s="14"/>
-      <c r="D76" s="18" t="str">
+      <c r="D76" s="18">
         <f>IF(NOT(ISBLANK($A76)),SUM(B$3:B76)-SUM(C$3:C76),"")</f>
-        <v/>
+        <v>532.96999999999935</v>
       </c>
       <c r="E76" s="7"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="18" t="str">
+      <c r="F76" s="14">
+        <v>52.66</v>
+      </c>
+      <c r="G76" s="18">
         <f>IF(NOT(ISBLANK($A76)),SUM(E$3:E76)-SUM(F$3:F76),"")</f>
-        <v/>
-      </c>
-      <c r="H76" s="8"/>
-      <c r="I76" s="20"/>
-      <c r="J76" s="8"/>
+        <v>-730.71000000000049</v>
+      </c>
+      <c r="H76" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" s="20">
+        <v>64709</v>
+      </c>
+      <c r="J76" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K76" s="22"/>
-      <c r="M76" s="38"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="11">
+        <v>42970</v>
+      </c>
       <c r="B77" s="7"/>
       <c r="C77" s="14"/>
-      <c r="D77" s="18" t="str">
+      <c r="D77" s="18">
         <f>IF(NOT(ISBLANK($A77)),SUM(B$3:B77)-SUM(C$3:C77),"")</f>
-        <v/>
+        <v>532.96999999999935</v>
       </c>
       <c r="E77" s="7"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="18" t="str">
+      <c r="F77" s="14">
+        <v>0.36</v>
+      </c>
+      <c r="G77" s="18">
         <f>IF(NOT(ISBLANK($A77)),SUM(E$3:E77)-SUM(F$3:F77),"")</f>
-        <v/>
-      </c>
-      <c r="H77" s="8"/>
-      <c r="I77" s="20"/>
-      <c r="J77" s="8"/>
+        <v>-731.07000000000016</v>
+      </c>
+      <c r="H77" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" s="20">
+        <v>65220</v>
+      </c>
+      <c r="J77" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K77" s="22"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="19" t="str">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="11">
+        <v>42970</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="18">
         <f>IF(NOT(ISBLANK($A78)),SUM(B$3:B78)-SUM(C$3:C78),"")</f>
-        <v/>
-      </c>
-      <c r="E78" s="9"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="19" t="str">
+        <v>532.96999999999935</v>
+      </c>
+      <c r="E78" s="7"/>
+      <c r="F78" s="14">
+        <v>53</v>
+      </c>
+      <c r="G78" s="18">
         <f>IF(NOT(ISBLANK($A78)),SUM(E$3:E78)-SUM(F$3:F78),"")</f>
-        <v/>
-      </c>
-      <c r="H78" s="10"/>
-      <c r="I78" s="21"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="23"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
+        <v>-784.07000000000016</v>
+      </c>
+      <c r="H78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" s="20">
+        <v>65220</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K78" s="22"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="12">
+        <v>42970</v>
+      </c>
       <c r="B79" s="9"/>
       <c r="C79" s="15"/>
-      <c r="D79" s="19" t="str">
+      <c r="D79" s="19">
         <f>IF(NOT(ISBLANK($A79)),SUM(B$3:B79)-SUM(C$3:C79),"")</f>
-        <v/>
+        <v>532.96999999999935</v>
       </c>
       <c r="E79" s="9"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="19" t="str">
+      <c r="F79" s="15">
+        <v>13.52</v>
+      </c>
+      <c r="G79" s="19">
         <f>IF(NOT(ISBLANK($A79)),SUM(E$3:E79)-SUM(F$3:F79),"")</f>
-        <v/>
+        <v>-797.5900000000006</v>
       </c>
       <c r="H79" s="10"/>
-      <c r="I79" s="21"/>
-      <c r="J79" s="10"/>
+      <c r="I79" s="21">
+        <v>65764</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="K79" s="23"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="12">
+        <v>42970</v>
+      </c>
       <c r="B80" s="9"/>
       <c r="C80" s="15"/>
-      <c r="D80" s="19" t="str">
+      <c r="D80" s="19">
         <f>IF(NOT(ISBLANK($A80)),SUM(B$3:B80)-SUM(C$3:C80),"")</f>
-        <v/>
+        <v>532.96999999999935</v>
       </c>
       <c r="E80" s="9"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="19" t="str">
+      <c r="F80" s="15">
+        <v>13.63</v>
+      </c>
+      <c r="G80" s="19">
         <f>IF(NOT(ISBLANK($A80)),SUM(E$3:E80)-SUM(F$3:F80),"")</f>
-        <v/>
-      </c>
-      <c r="H80" s="10"/>
-      <c r="I80" s="21"/>
-      <c r="J80" s="10"/>
+        <v>-811.22000000000071</v>
+      </c>
+      <c r="H80" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="21">
+        <v>65764</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="18" t="str">
+      <c r="A81" s="12">
+        <v>42971</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="15">
+        <v>222.42</v>
+      </c>
+      <c r="D81" s="19">
         <f>IF(NOT(ISBLANK($A81)),SUM(B$3:B81)-SUM(C$3:C81),"")</f>
-        <v/>
-      </c>
-      <c r="E81" s="7"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="18" t="str">
+        <v>310.54999999999927</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="19">
         <f>IF(NOT(ISBLANK($A81)),SUM(E$3:E81)-SUM(F$3:F81),"")</f>
-        <v/>
-      </c>
-      <c r="H81" s="8"/>
-      <c r="I81" s="20"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="22"/>
+        <v>-811.22000000000071</v>
+      </c>
+      <c r="H81" s="10"/>
+      <c r="I81" s="21"/>
+      <c r="J81" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K81" s="23"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="11">
+        <v>42974</v>
+      </c>
       <c r="B82" s="7"/>
       <c r="C82" s="14"/>
-      <c r="D82" s="18" t="str">
+      <c r="D82" s="18">
         <f>IF(NOT(ISBLANK($A82)),SUM(B$3:B82)-SUM(C$3:C82),"")</f>
-        <v/>
+        <v>310.54999999999927</v>
       </c>
       <c r="E82" s="7"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="18" t="str">
+      <c r="F82" s="14">
+        <v>38.4</v>
+      </c>
+      <c r="G82" s="18">
         <f>IF(NOT(ISBLANK($A82)),SUM(E$3:E82)-SUM(F$3:F82),"")</f>
-        <v/>
-      </c>
-      <c r="H82" s="8"/>
-      <c r="I82" s="20"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="22"/>
+        <v>-849.62000000000035</v>
+      </c>
+      <c r="H82" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" s="20">
+        <v>65764</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K82" s="39" t="str">
+        <f>"Car wash portion:"&amp;TEXT(F82-22.59,"$#,##0.00")</f>
+        <v>Car wash portion:$15.81</v>
+      </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="11">
+        <v>42976</v>
+      </c>
       <c r="B83" s="7"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="18" t="str">
+      <c r="C83" s="14">
+        <v>310.55</v>
+      </c>
+      <c r="D83" s="18">
         <f>IF(NOT(ISBLANK($A83)),SUM(B$3:B83)-SUM(C$3:C83),"")</f>
-        <v/>
-      </c>
-      <c r="E83" s="7"/>
+        <v>-9.0949470177292824E-13</v>
+      </c>
+      <c r="E83" s="7">
+        <v>310.55</v>
+      </c>
       <c r="F83" s="14"/>
-      <c r="G83" s="18" t="str">
+      <c r="G83" s="18">
         <f>IF(NOT(ISBLANK($A83)),SUM(E$3:E83)-SUM(F$3:F83),"")</f>
-        <v/>
+        <v>-539.07000000000016</v>
       </c>
       <c r="H83" s="8"/>
       <c r="I83" s="20"/>
-      <c r="J83" s="8"/>
+      <c r="J83" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="K83" s="22"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="19" t="str">
+      <c r="A84" s="11"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="18" t="str">
         <f>IF(NOT(ISBLANK($A84)),SUM(B$3:B84)-SUM(C$3:C84),"")</f>
         <v/>
       </c>
-      <c r="E84" s="9"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="19" t="str">
+      <c r="E84" s="7"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="18" t="str">
         <f>IF(NOT(ISBLANK($A84)),SUM(E$3:E84)-SUM(F$3:F84),"")</f>
         <v/>
       </c>
-      <c r="H84" s="10"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="10"/>
-      <c r="K84" s="23"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="22"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
@@ -3003,23 +3133,23 @@
       <c r="K86" s="23"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="18" t="str">
+      <c r="A87" s="12"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="19" t="str">
         <f>IF(NOT(ISBLANK($A87)),SUM(B$3:B87)-SUM(C$3:C87),"")</f>
         <v/>
       </c>
-      <c r="E87" s="7"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="18" t="str">
+      <c r="E87" s="9"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="19" t="str">
         <f>IF(NOT(ISBLANK($A87)),SUM(E$3:E87)-SUM(F$3:F87),"")</f>
         <v/>
       </c>
-      <c r="H87" s="8"/>
-      <c r="I87" s="20"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="22"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="23"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
@@ -3060,23 +3190,23 @@
       <c r="K89" s="22"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="19" t="str">
+      <c r="A90" s="11"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="18" t="str">
         <f>IF(NOT(ISBLANK($A90)),SUM(B$3:B90)-SUM(C$3:C90),"")</f>
         <v/>
       </c>
-      <c r="E90" s="9"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="19" t="str">
+      <c r="E90" s="7"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="18" t="str">
         <f>IF(NOT(ISBLANK($A90)),SUM(E$3:E90)-SUM(F$3:F90),"")</f>
         <v/>
       </c>
-      <c r="H90" s="10"/>
-      <c r="I90" s="21"/>
-      <c r="J90" s="10"/>
-      <c r="K90" s="23"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="22"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
@@ -3117,23 +3247,23 @@
       <c r="K92" s="23"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="11"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="18" t="str">
+      <c r="A93" s="12"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="19" t="str">
         <f>IF(NOT(ISBLANK($A93)),SUM(B$3:B93)-SUM(C$3:C93),"")</f>
         <v/>
       </c>
-      <c r="E93" s="7"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="18" t="str">
+      <c r="E93" s="9"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="19" t="str">
         <f>IF(NOT(ISBLANK($A93)),SUM(E$3:E93)-SUM(F$3:F93),"")</f>
         <v/>
       </c>
-      <c r="H93" s="8"/>
-      <c r="I93" s="20"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="22"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="23"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
@@ -3174,23 +3304,23 @@
       <c r="K95" s="22"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="19" t="str">
+      <c r="A96" s="11"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="18" t="str">
         <f>IF(NOT(ISBLANK($A96)),SUM(B$3:B96)-SUM(C$3:C96),"")</f>
         <v/>
       </c>
-      <c r="E96" s="9"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="19" t="str">
+      <c r="E96" s="7"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="18" t="str">
         <f>IF(NOT(ISBLANK($A96)),SUM(E$3:E96)-SUM(F$3:F96),"")</f>
         <v/>
       </c>
-      <c r="H96" s="10"/>
-      <c r="I96" s="21"/>
-      <c r="J96" s="10"/>
-      <c r="K96" s="23"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="22"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
@@ -3231,23 +3361,23 @@
       <c r="K98" s="23"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="18" t="str">
+      <c r="A99" s="12"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="19" t="str">
         <f>IF(NOT(ISBLANK($A99)),SUM(B$3:B99)-SUM(C$3:C99),"")</f>
         <v/>
       </c>
-      <c r="E99" s="7"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="18" t="str">
+      <c r="E99" s="9"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="19" t="str">
         <f>IF(NOT(ISBLANK($A99)),SUM(E$3:E99)-SUM(F$3:F99),"")</f>
         <v/>
       </c>
-      <c r="H99" s="8"/>
-      <c r="I99" s="20"/>
-      <c r="J99" s="8"/>
-      <c r="K99" s="22"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="21"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="23"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
@@ -3288,93 +3418,54 @@
       <c r="K101" s="22"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A102)),SUM(B$3:B102)-SUM(C$3:C102),"")</f>
-        <v/>
-      </c>
-      <c r="E102" s="9"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A102)),SUM(E$3:E102)-SUM(F$3:F102),"")</f>
-        <v/>
-      </c>
-      <c r="H102" s="10"/>
-      <c r="I102" s="21"/>
-      <c r="J102" s="10"/>
-      <c r="K102" s="23"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="20"/>
+      <c r="J102" s="8"/>
+      <c r="K102" s="22"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="9"/>
       <c r="C103" s="15"/>
-      <c r="D103" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A103)),SUM(B$3:B103)-SUM(C$3:C103),"")</f>
-        <v/>
-      </c>
+      <c r="D103" s="19"/>
       <c r="E103" s="9"/>
       <c r="F103" s="15"/>
-      <c r="G103" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A103)),SUM(E$3:E103)-SUM(F$3:F103),"")</f>
-        <v/>
-      </c>
+      <c r="G103" s="19"/>
       <c r="H103" s="10"/>
       <c r="I103" s="21"/>
       <c r="J103" s="10"/>
       <c r="K103" s="23"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A104)),SUM(B$3:B104)-SUM(C$3:C104),"")</f>
-        <v/>
-      </c>
-      <c r="E104" s="9"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="19" t="str">
-        <f>IF(NOT(ISBLANK($A104)),SUM(E$3:E104)-SUM(F$3:F104),"")</f>
-        <v/>
-      </c>
-      <c r="H104" s="10"/>
-      <c r="I104" s="21"/>
-      <c r="J104" s="10"/>
-      <c r="K104" s="23"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="18" t="str">
-        <f>IF(NOT(ISBLANK($A105)),SUM(B$3:B105)-SUM(C$3:C105),"")</f>
-        <v/>
-      </c>
-      <c r="E105" s="7"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="18" t="str">
-        <f>IF(NOT(ISBLANK($A105)),SUM(E$3:E105)-SUM(F$3:F105),"")</f>
-        <v/>
-      </c>
-      <c r="H105" s="8"/>
-      <c r="I105" s="20"/>
-      <c r="J105" s="8"/>
-      <c r="K105" s="22"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="2"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="20"/>
-      <c r="J106" s="8"/>
-      <c r="K106" s="22"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
@@ -4336,41 +4427,9 @@
       <c r="F226" s="16"/>
       <c r="G226" s="2"/>
     </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B227" s="1"/>
-      <c r="C227" s="16"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="1"/>
-      <c r="F227" s="16"/>
-      <c r="G227" s="2"/>
-    </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B228" s="1"/>
-      <c r="C228" s="16"/>
-      <c r="D228" s="2"/>
-      <c r="E228" s="1"/>
-      <c r="F228" s="16"/>
-      <c r="G228" s="2"/>
-    </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="1"/>
-      <c r="C229" s="16"/>
-      <c r="D229" s="2"/>
-      <c r="E229" s="1"/>
-      <c r="F229" s="16"/>
-      <c r="G229" s="2"/>
-    </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B230" s="1"/>
-      <c r="C230" s="16"/>
-      <c r="D230" s="2"/>
-      <c r="E230" s="1"/>
-      <c r="F230" s="16"/>
-      <c r="G230" s="2"/>
-    </row>
   </sheetData>
-  <sortState ref="A52:K71">
-    <sortCondition ref="A52:A71"/>
+  <sortState ref="A69:O81">
+    <sortCondition ref="A69:A81"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="I1:I2"/>

</xml_diff>

<commit_message>
Added the swim budgeting work shhet and semi-monthly transfers.
</commit_message>
<xml_diff>
--- a/book-keeping.xlsx
+++ b/book-keeping.xlsx
@@ -4,22 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28755" windowHeight="5955"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28755" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="Car" sheetId="1" r:id="rId1"/>
     <sheet name="Swimming" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Swim Budget" sheetId="4" r:id="rId3"/>
+    <sheet name="Semi-Monthly Transfers" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Car!$A$1:$K$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Car!$A$1:$K$102</definedName>
+    <definedName name="already_paid">'Swim Budget'!$A$42</definedName>
+    <definedName name="annual_budget">'Swim Budget'!$A$41</definedName>
+    <definedName name="hotel_cost">'Swim Budget'!$A$36</definedName>
+    <definedName name="installments_remain">'Swim Budget'!$A$43</definedName>
+    <definedName name="US_training_camp">'Swim Budget'!$F$48</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="130">
   <si>
     <t>Date</t>
   </si>
@@ -162,19 +168,271 @@
     <t>Oil Change</t>
   </si>
   <si>
-    <t>Minimum Balance</t>
+    <t>ROCS Account</t>
+  </si>
+  <si>
+    <t>Equipment/Expenses (Visa)</t>
+  </si>
+  <si>
+    <t>Goggle and Mesh Bag (x2) from GoSwim</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Flippers</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Dinner and Movie</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Ankle Strap, kick board, pull bouy</t>
+  </si>
+  <si>
+    <t>Maximum Transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All in </t>
+  </si>
+  <si>
+    <t>Training Camp</t>
+  </si>
+  <si>
+    <t>Per Day</t>
+  </si>
+  <si>
+    <t>YOW</t>
+  </si>
+  <si>
+    <t>YWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tickets </t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Quality Inn &amp; Suites, 635 Pembina Hwy (closer - 30 minute walk)</t>
+  </si>
+  <si>
+    <t>Check Out:</t>
+  </si>
+  <si>
+    <t>Check In:</t>
+  </si>
+  <si>
+    <t>Holiday Inn Winnipeg South</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Junior Nationals</t>
+  </si>
+  <si>
+    <t>Winnipeg</t>
+  </si>
+  <si>
+    <t>Per Trip</t>
+  </si>
+  <si>
+    <t>Cabs</t>
+  </si>
+  <si>
+    <t>YQG</t>
+  </si>
+  <si>
+    <t>Per Person</t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>Total Points</t>
+  </si>
+  <si>
+    <t>Points per Night</t>
+  </si>
+  <si>
+    <t>ETR</t>
+  </si>
+  <si>
+    <t>Total Number of Nights</t>
+  </si>
+  <si>
+    <t>1800km @ 8l/100km @ $1.30 /l per trip</t>
+  </si>
+  <si>
+    <t>Driving</t>
+  </si>
+  <si>
+    <t>Hotel Nights</t>
+  </si>
+  <si>
+    <t>Best Western Plus Waterfront Windsor (across the street)</t>
+  </si>
+  <si>
+    <t>Holiday Inn Windsor Downtown (&lt; 10 minute walk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel </t>
+  </si>
+  <si>
+    <t>Eastern Championships</t>
+  </si>
+  <si>
+    <t>Windsor</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Trips to Toronto</t>
+  </si>
+  <si>
+    <t>Person Days in Toronto</t>
+  </si>
+  <si>
+    <t>Spring Championships, Summer Festival, Summer Championships</t>
+  </si>
+  <si>
+    <t>Grocery</t>
+  </si>
+  <si>
+    <t>Per Day/Per person</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>1000km @ 8l/100km @ $1.30 /l per trip</t>
+  </si>
+  <si>
+    <t>Crowne Plaza Toronto Airport, 33 Carlson Ct, Etobicoke, ON</t>
+  </si>
+  <si>
+    <t>Toronto Airport Marriott Hotel, Dixon Road, Etobicoke, ON</t>
+  </si>
+  <si>
+    <t>Hotel Suggestions</t>
+  </si>
+  <si>
+    <t>Summer Championships</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express, 10 East Pearce Street, Richmond Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toronto Meets </t>
+  </si>
+  <si>
+    <t>Staybridge Suites Toronto-Markham, 355 South Park Rd, Thornhill</t>
+  </si>
+  <si>
+    <t>Summer Festival</t>
+  </si>
+  <si>
+    <t>Olivier Skiing</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Spring Championships</t>
+  </si>
+  <si>
+    <t>meet fees</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Belleville</t>
+  </si>
+  <si>
+    <t>Point Claire</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>So far</t>
+  </si>
+  <si>
+    <t>Payments Remaining</t>
+  </si>
+  <si>
+    <t>Cost per Night</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Twice Monthly Budget</t>
+  </si>
+  <si>
+    <t>No Hotels</t>
+  </si>
+  <si>
+    <t>With Hotels</t>
+  </si>
+  <si>
+    <t>RRSP</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Pets</t>
+  </si>
+  <si>
+    <t>Visa Transfer</t>
+  </si>
+  <si>
+    <t>House</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="9">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode=";;;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +469,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +569,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -400,15 +764,282 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,21 +1048,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,17 +1072,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,13 +1099,202 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="6" fontId="5" fillId="4" borderId="20" xfId="3" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="20" xfId="3" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="15" xfId="3" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="10" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="7" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="6" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="11" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="20" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="169" fontId="5" fillId="4" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="13" fillId="5" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="4" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="18" xfId="7" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="8" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="35" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="5" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="5" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="36" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="4" borderId="34" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="9">
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency 2" xfId="8"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="5" builtinId="24"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="7" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -481,6 +1302,76 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$L$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4097" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4097"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Tahoma"/>
+                  <a:ea typeface="Tahoma"/>
+                  <a:cs typeface="Tahoma"/>
+                </a:rPr>
+                <a:t>Early Check in?</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,17 +1661,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P226"/>
+  <dimension ref="A1:R227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A52" activePane="bottomLeft"/>
-      <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+      <pane ySplit="900" topLeftCell="A64" activePane="bottomLeft"/>
+      <selection activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -793,30 +1684,30 @@
     <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
@@ -826,9 +1717,13 @@
         <v>222.42</v>
       </c>
       <c r="O1" s="32"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+      <c r="R1" s="34">
+        <f>SUM(B$3:B201)-SUM(C$3:C201)-N1</f>
+        <v>-8.2422957348171622E-13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -847,10 +1742,10 @@
       <c r="G2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
       <c r="M2" t="s">
         <v>14</v>
       </c>
@@ -862,10 +1757,14 @@
         <v>305.39</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="R2" s="34">
+        <f>SUM(B$3:B201)-SUM(C$3:C201)-O2</f>
+        <v>-82.970000000000823</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>42856</v>
       </c>
@@ -892,7 +1791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>42875</v>
       </c>
@@ -921,7 +1820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>42877</v>
       </c>
@@ -948,7 +1847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>42878</v>
       </c>
@@ -979,7 +1878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>42879</v>
       </c>
@@ -1006,7 +1905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>42881</v>
       </c>
@@ -1033,7 +1932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>42870</v>
       </c>
@@ -1058,7 +1957,7 @@
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>42882</v>
       </c>
@@ -1081,7 +1980,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>42882</v>
       </c>
@@ -1106,7 +2005,7 @@
       </c>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>42884</v>
       </c>
@@ -1133,7 +2032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>42884</v>
       </c>
@@ -1160,7 +2059,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42886</v>
       </c>
@@ -1189,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>42886</v>
       </c>
@@ -1218,7 +2117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>42887</v>
       </c>
@@ -2798,55 +3697,57 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
-        <v>42958</v>
-      </c>
-      <c r="B74" s="9"/>
+        <v>42962</v>
+      </c>
+      <c r="B74" s="9">
+        <v>450</v>
+      </c>
       <c r="C74" s="15"/>
       <c r="D74" s="19">
-        <f>IF(NOT(ISBLANK($A74)),SUM(B$3:B74)-SUM(C$3:C74),"")</f>
-        <v>82.969999999999345</v>
+        <f>IF(NOT(ISBLANK($A74)),SUM(B$3:B75)-SUM(C$3:C75),"")</f>
+        <v>532.96999999999935</v>
       </c>
       <c r="E74" s="9"/>
-      <c r="F74" s="15">
-        <v>187.58</v>
-      </c>
+      <c r="F74" s="15"/>
       <c r="G74" s="19">
-        <f>IF(NOT(ISBLANK($A74)),SUM(E$3:E74)-SUM(F$3:F74),"")</f>
+        <f>IF(NOT(ISBLANK($A74)),SUM(E$3:E75)-SUM(F$3:F75),"")</f>
         <v>-678.05000000000018</v>
       </c>
-      <c r="H74" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="H74" s="10"/>
       <c r="I74" s="21"/>
       <c r="J74" s="10" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="K74" s="23"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="12">
-        <v>42962</v>
-      </c>
-      <c r="B75" s="9">
-        <v>450</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="19">
+      <c r="A75" s="11">
+        <v>42964</v>
+      </c>
+      <c r="B75" s="7"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="18">
         <f>IF(NOT(ISBLANK($A75)),SUM(B$3:B75)-SUM(C$3:C75),"")</f>
         <v>532.96999999999935</v>
       </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="19">
+      <c r="E75" s="7"/>
+      <c r="F75" s="14">
+        <v>187.58</v>
+      </c>
+      <c r="G75" s="18">
         <f>IF(NOT(ISBLANK($A75)),SUM(E$3:E75)-SUM(F$3:F75),"")</f>
         <v>-678.05000000000018</v>
       </c>
-      <c r="H75" s="10"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K75" s="23"/>
+      <c r="H75" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" s="20">
+        <v>64493</v>
+      </c>
+      <c r="J75" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K75" s="22"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
@@ -2907,33 +3808,33 @@
       <c r="K77" s="22"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="11">
+      <c r="A78" s="12">
         <v>42970</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="18">
+      <c r="B78" s="9"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="19">
         <f>IF(NOT(ISBLANK($A78)),SUM(B$3:B78)-SUM(C$3:C78),"")</f>
         <v>532.96999999999935</v>
       </c>
-      <c r="E78" s="7"/>
-      <c r="F78" s="14">
+      <c r="E78" s="9"/>
+      <c r="F78" s="15">
         <v>53</v>
       </c>
-      <c r="G78" s="18">
+      <c r="G78" s="19">
         <f>IF(NOT(ISBLANK($A78)),SUM(E$3:E78)-SUM(F$3:F78),"")</f>
         <v>-784.07000000000016</v>
       </c>
-      <c r="H78" s="8" t="b">
+      <c r="H78" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I78" s="20">
+      <c r="I78" s="21">
         <v>65220</v>
       </c>
-      <c r="J78" s="8" t="s">
+      <c r="J78" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K78" s="22"/>
+      <c r="K78" s="23"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
@@ -2953,7 +3854,9 @@
         <f>IF(NOT(ISBLANK($A79)),SUM(E$3:E79)-SUM(F$3:F79),"")</f>
         <v>-797.5900000000006</v>
       </c>
-      <c r="H79" s="10"/>
+      <c r="H79" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="I79" s="21">
         <v>65764</v>
       </c>
@@ -2992,29 +3895,29 @@
       <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="12">
+      <c r="A81" s="11">
         <v>42971</v>
       </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="15">
+      <c r="B81" s="7"/>
+      <c r="C81" s="14">
         <v>222.42</v>
       </c>
-      <c r="D81" s="19">
+      <c r="D81" s="18">
         <f>IF(NOT(ISBLANK($A81)),SUM(B$3:B81)-SUM(C$3:C81),"")</f>
         <v>310.54999999999927</v>
       </c>
-      <c r="E81" s="9"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="19">
+      <c r="E81" s="7"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="18">
         <f>IF(NOT(ISBLANK($A81)),SUM(E$3:E81)-SUM(F$3:F81),"")</f>
         <v>-811.22000000000071</v>
       </c>
-      <c r="H81" s="10"/>
-      <c r="I81" s="21"/>
-      <c r="J81" s="10" t="s">
+      <c r="H81" s="8"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K81" s="23"/>
+      <c r="K81" s="22"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
@@ -3043,7 +3946,7 @@
       <c r="J82" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K82" s="39" t="str">
+      <c r="K82" s="22" t="str">
         <f>"Car wash portion:"&amp;TEXT(F82-22.59,"$#,##0.00")</f>
         <v>Car wash portion:$15.81</v>
       </c>
@@ -3076,194 +3979,270 @@
       <c r="K83" s="22"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="18" t="str">
+      <c r="A84" s="12">
+        <v>42977</v>
+      </c>
+      <c r="B84" s="9">
+        <v>450</v>
+      </c>
+      <c r="C84" s="15"/>
+      <c r="D84" s="19">
         <f>IF(NOT(ISBLANK($A84)),SUM(B$3:B84)-SUM(C$3:C84),"")</f>
-        <v/>
-      </c>
-      <c r="E84" s="7"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="18" t="str">
+        <v>449.99999999999909</v>
+      </c>
+      <c r="E84" s="9"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="19">
         <f>IF(NOT(ISBLANK($A84)),SUM(E$3:E84)-SUM(F$3:F84),"")</f>
-        <v/>
-      </c>
-      <c r="H84" s="8"/>
-      <c r="I84" s="20"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="22"/>
+        <v>-539.07000000000016</v>
+      </c>
+      <c r="H84" s="10"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K84" s="23"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
+      <c r="A85" s="12">
+        <v>42983</v>
+      </c>
       <c r="B85" s="9"/>
       <c r="C85" s="15"/>
-      <c r="D85" s="19" t="str">
+      <c r="D85" s="19">
         <f>IF(NOT(ISBLANK($A85)),SUM(B$3:B85)-SUM(C$3:C85),"")</f>
-        <v/>
+        <v>449.99999999999909</v>
       </c>
       <c r="E85" s="9"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="19" t="str">
+      <c r="F85" s="15">
+        <v>3</v>
+      </c>
+      <c r="G85" s="19">
         <f>IF(NOT(ISBLANK($A85)),SUM(E$3:E85)-SUM(F$3:F85),"")</f>
-        <v/>
+        <v>-542.07000000000016</v>
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="21"/>
-      <c r="J85" s="10"/>
+      <c r="J85" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="K85" s="23"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
+      <c r="A86" s="12">
+        <v>42983</v>
+      </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="19" t="str">
+      <c r="C86" s="15">
+        <v>144.61000000000001</v>
+      </c>
+      <c r="D86" s="19">
         <f>IF(NOT(ISBLANK($A86)),SUM(B$3:B86)-SUM(C$3:C86),"")</f>
-        <v/>
-      </c>
-      <c r="E86" s="9"/>
+        <v>305.38999999999942</v>
+      </c>
+      <c r="E86" s="9">
+        <v>144.61000000000001</v>
+      </c>
       <c r="F86" s="15"/>
-      <c r="G86" s="19" t="str">
+      <c r="G86" s="19">
         <f>IF(NOT(ISBLANK($A86)),SUM(E$3:E86)-SUM(F$3:F86),"")</f>
-        <v/>
+        <v>-397.46000000000004</v>
       </c>
       <c r="H86" s="10"/>
       <c r="I86" s="21"/>
-      <c r="J86" s="10"/>
+      <c r="J86" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="K86" s="23"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="19" t="str">
+      <c r="A87" s="11">
+        <v>42985</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="14">
+        <v>82.97</v>
+      </c>
+      <c r="D87" s="18">
         <f>IF(NOT(ISBLANK($A87)),SUM(B$3:B87)-SUM(C$3:C87),"")</f>
-        <v/>
-      </c>
-      <c r="E87" s="9"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="19" t="str">
+        <v>222.41999999999916</v>
+      </c>
+      <c r="E87" s="7"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="18">
         <f>IF(NOT(ISBLANK($A87)),SUM(E$3:E87)-SUM(F$3:F87),"")</f>
-        <v/>
-      </c>
-      <c r="H87" s="10"/>
-      <c r="I87" s="21"/>
-      <c r="J87" s="10"/>
-      <c r="K87" s="23"/>
+        <v>-397.46000000000004</v>
+      </c>
+      <c r="H87" s="8"/>
+      <c r="I87" s="20"/>
+      <c r="J87" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K87" s="22"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+      <c r="A88" s="11">
+        <v>42985</v>
+      </c>
       <c r="B88" s="7"/>
       <c r="C88" s="14"/>
-      <c r="D88" s="18" t="str">
+      <c r="D88" s="18">
         <f>IF(NOT(ISBLANK($A88)),SUM(B$3:B88)-SUM(C$3:C88),"")</f>
-        <v/>
+        <v>222.41999999999916</v>
       </c>
       <c r="E88" s="7"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="18" t="str">
+      <c r="F88" s="14">
+        <v>75</v>
+      </c>
+      <c r="G88" s="18">
         <f>IF(NOT(ISBLANK($A88)),SUM(E$3:E88)-SUM(F$3:F88),"")</f>
-        <v/>
-      </c>
-      <c r="H88" s="8"/>
-      <c r="I88" s="20"/>
-      <c r="J88" s="8"/>
+        <v>-472.46000000000004</v>
+      </c>
+      <c r="H88" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" s="20">
+        <v>66364</v>
+      </c>
+      <c r="J88" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K88" s="22"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
+      <c r="A89" s="11">
+        <v>42987</v>
+      </c>
       <c r="B89" s="7"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="18" t="str">
+      <c r="C89" s="14">
+        <v>222.42</v>
+      </c>
+      <c r="D89" s="18">
         <f>IF(NOT(ISBLANK($A89)),SUM(B$3:B89)-SUM(C$3:C89),"")</f>
-        <v/>
+        <v>-9.0949470177292824E-13</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="14"/>
-      <c r="G89" s="18" t="str">
+      <c r="G89" s="18">
         <f>IF(NOT(ISBLANK($A89)),SUM(E$3:E89)-SUM(F$3:F89),"")</f>
-        <v/>
+        <v>-472.46000000000004</v>
       </c>
       <c r="H89" s="8"/>
       <c r="I89" s="20"/>
-      <c r="J89" s="8"/>
+      <c r="J89" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="K89" s="22"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="18" t="str">
+      <c r="A90" s="12">
+        <v>42992</v>
+      </c>
+      <c r="B90" s="9"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="19">
         <f>IF(NOT(ISBLANK($A90)),SUM(B$3:B90)-SUM(C$3:C90),"")</f>
-        <v/>
-      </c>
-      <c r="E90" s="7"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="18" t="str">
+        <v>-9.0949470177292824E-13</v>
+      </c>
+      <c r="E90" s="9"/>
+      <c r="F90" s="15">
+        <v>42.93</v>
+      </c>
+      <c r="G90" s="19">
         <f>IF(NOT(ISBLANK($A90)),SUM(E$3:E90)-SUM(F$3:F90),"")</f>
-        <v/>
-      </c>
-      <c r="H90" s="8"/>
-      <c r="I90" s="20"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="22"/>
+        <v>-515.39000000000033</v>
+      </c>
+      <c r="H90" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I90" s="21">
+        <v>66796</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K90" s="23"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
+      <c r="A91" s="12">
+        <v>42995</v>
+      </c>
       <c r="B91" s="9"/>
       <c r="C91" s="15"/>
-      <c r="D91" s="19" t="str">
+      <c r="D91" s="19">
         <f>IF(NOT(ISBLANK($A91)),SUM(B$3:B91)-SUM(C$3:C91),"")</f>
-        <v/>
+        <v>-9.0949470177292824E-13</v>
       </c>
       <c r="E91" s="9"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="19" t="str">
+      <c r="F91" s="15">
+        <v>67</v>
+      </c>
+      <c r="G91" s="19">
         <f>IF(NOT(ISBLANK($A91)),SUM(E$3:E91)-SUM(F$3:F91),"")</f>
-        <v/>
-      </c>
-      <c r="H91" s="10"/>
-      <c r="I91" s="21"/>
-      <c r="J91" s="10"/>
+        <v>-582.39000000000033</v>
+      </c>
+      <c r="H91" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I91" s="21">
+        <v>66883</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="K91" s="23"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="9"/>
+      <c r="A92" s="12">
+        <v>42996</v>
+      </c>
+      <c r="B92" s="9">
+        <v>450</v>
+      </c>
       <c r="C92" s="15"/>
-      <c r="D92" s="19" t="str">
+      <c r="D92" s="19">
         <f>IF(NOT(ISBLANK($A92)),SUM(B$3:B92)-SUM(C$3:C92),"")</f>
-        <v/>
+        <v>449.99999999999909</v>
       </c>
       <c r="E92" s="9"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="19" t="str">
+      <c r="G92" s="19">
         <f>IF(NOT(ISBLANK($A92)),SUM(E$3:E92)-SUM(F$3:F92),"")</f>
-        <v/>
+        <v>-582.39000000000033</v>
       </c>
       <c r="H92" s="10"/>
       <c r="I92" s="21"/>
-      <c r="J92" s="10"/>
+      <c r="J92" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K92" s="23"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="19" t="str">
+      <c r="A93" s="11">
+        <v>42996</v>
+      </c>
+      <c r="B93" s="7"/>
+      <c r="C93" s="14">
+        <v>227.58</v>
+      </c>
+      <c r="D93" s="18">
         <f>IF(NOT(ISBLANK($A93)),SUM(B$3:B93)-SUM(C$3:C93),"")</f>
-        <v/>
-      </c>
-      <c r="E93" s="9"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="19" t="str">
+        <v>222.41999999999916</v>
+      </c>
+      <c r="E93" s="7">
+        <v>227.58</v>
+      </c>
+      <c r="F93" s="14"/>
+      <c r="G93" s="18">
         <f>IF(NOT(ISBLANK($A93)),SUM(E$3:E93)-SUM(F$3:F93),"")</f>
-        <v/>
-      </c>
-      <c r="H93" s="10"/>
-      <c r="I93" s="21"/>
-      <c r="J93" s="10"/>
-      <c r="K93" s="23"/>
+        <v>-354.8100000000004</v>
+      </c>
+      <c r="H93" s="8"/>
+      <c r="I93" s="20"/>
+      <c r="J93" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K93" s="22"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
@@ -3304,23 +4283,23 @@
       <c r="K95" s="22"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="18" t="str">
+      <c r="A96" s="12"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="19" t="str">
         <f>IF(NOT(ISBLANK($A96)),SUM(B$3:B96)-SUM(C$3:C96),"")</f>
         <v/>
       </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="18" t="str">
+      <c r="E96" s="9"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="19" t="str">
         <f>IF(NOT(ISBLANK($A96)),SUM(E$3:E96)-SUM(F$3:F96),"")</f>
         <v/>
       </c>
-      <c r="H96" s="8"/>
-      <c r="I96" s="20"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="22"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="23"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
@@ -3361,23 +4340,23 @@
       <c r="K98" s="23"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="19" t="str">
+      <c r="A99" s="11"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="18" t="str">
         <f>IF(NOT(ISBLANK($A99)),SUM(B$3:B99)-SUM(C$3:C99),"")</f>
         <v/>
       </c>
-      <c r="E99" s="9"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="19" t="str">
+      <c r="E99" s="7"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="18" t="str">
         <f>IF(NOT(ISBLANK($A99)),SUM(E$3:E99)-SUM(F$3:F99),"")</f>
         <v/>
       </c>
-      <c r="H99" s="10"/>
-      <c r="I99" s="21"/>
-      <c r="J99" s="10"/>
-      <c r="K99" s="23"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="20"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="22"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
@@ -3418,17 +4397,23 @@
       <c r="K101" s="22"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="18"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="20"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="22"/>
+      <c r="A102" s="12"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="19" t="str">
+        <f>IF(NOT(ISBLANK($A102)),SUM(B$3:B102)-SUM(C$3:C102),"")</f>
+        <v/>
+      </c>
+      <c r="E102" s="9"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="19" t="str">
+        <f>IF(NOT(ISBLANK($A102)),SUM(E$3:E102)-SUM(F$3:F102),"")</f>
+        <v/>
+      </c>
+      <c r="H102" s="10"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="10"/>
+      <c r="K102" s="23"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
@@ -3444,12 +4429,17 @@
       <c r="K103" s="23"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="1"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="16"/>
-      <c r="G104" s="2"/>
+      <c r="A104" s="12"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="21"/>
+      <c r="J104" s="10"/>
+      <c r="K104" s="23"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
@@ -4426,6 +5416,14 @@
       <c r="E226" s="1"/>
       <c r="F226" s="16"/>
       <c r="G226" s="2"/>
+    </row>
+    <row r="227" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B227" s="1"/>
+      <c r="C227" s="16"/>
+      <c r="D227" s="2"/>
+      <c r="E227" s="1"/>
+      <c r="F227" s="16"/>
+      <c r="G227" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A69:O81">
@@ -4447,24 +5445,1819 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>42979</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="18">
+        <f>IF(NOT(ISBLANK($A3)),SUM(B$3:B3)-SUM(C$3:C3),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="18">
+        <f>IF(NOT(ISBLANK($A3)),SUM(E$3:E3)-SUM(F$3:F3),"")</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="14">
+        <v>2862.19</v>
+      </c>
+      <c r="J3" s="18">
+        <f>IF(NOT(ISBLANK($A3)),SUM(H$3:H3)-SUM(I$3:I3),"")</f>
+        <v>-2862.19</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>42979</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="18">
+        <f>IF(NOT(ISBLANK($A4)),SUM(B$3:B4)-SUM(C$3:C4),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="14">
+        <v>103.96</v>
+      </c>
+      <c r="G4" s="18">
+        <f>IF(NOT(ISBLANK($A4)),SUM(E$3:E4)-SUM(F$3:F4),"")</f>
+        <v>-103.96</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="18">
+        <f>IF(NOT(ISBLANK($A4)),SUM(H$3:H4)-SUM(I$3:I4),"")</f>
+        <v>-2862.19</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>42980</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="18">
+        <f>IF(NOT(ISBLANK($A5)),SUM(B$3:B5)-SUM(C$3:C5),"")</f>
+        <v>3000</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="18">
+        <f>IF(NOT(ISBLANK($A5)),SUM(E$3:E5)-SUM(F$3:F5),"")</f>
+        <v>-103.96</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="18">
+        <f>IF(NOT(ISBLANK($A5)),SUM(H$3:H5)-SUM(I$3:I5),"")</f>
+        <v>-2862.19</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>42980</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="14">
+        <v>103.96</v>
+      </c>
+      <c r="D6" s="18">
+        <f>IF(NOT(ISBLANK($A6)),SUM(B$3:B6)-SUM(C$3:C6),"")</f>
+        <v>2896.04</v>
+      </c>
+      <c r="E6" s="7">
+        <v>103.96</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="18">
+        <f>IF(NOT(ISBLANK($A6)),SUM(E$3:E6)-SUM(F$3:F6),"")</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="18">
+        <f>IF(NOT(ISBLANK($A6)),SUM(H$3:H6)-SUM(I$3:I6),"")</f>
+        <v>-2862.19</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>42983</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="14">
+        <v>2862.19</v>
+      </c>
+      <c r="D7" s="18">
+        <f>IF(NOT(ISBLANK($A7)),SUM(B$3:B7)-SUM(C$3:C7),"")</f>
+        <v>33.849999999999909</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="18">
+        <f>IF(NOT(ISBLANK($A7)),SUM(E$3:E7)-SUM(F$3:F7),"")</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2862.19</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="18">
+        <f>IF(NOT(ISBLANK($A7)),SUM(H$3:H7)-SUM(I$3:I7),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>42984</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="18">
+        <f>IF(NOT(ISBLANK($A8)),SUM(B$3:B8)-SUM(C$3:C8),"")</f>
+        <v>33.849999999999909</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="14">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="G8" s="18">
+        <f>IF(NOT(ISBLANK($A8)),SUM(E$3:E8)-SUM(F$3:F8),"")</f>
+        <v>-36.160000000000011</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="18">
+        <f>IF(NOT(ISBLANK($A8)),SUM(H$3:H8)-SUM(I$3:I8),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>42986</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="18">
+        <f>IF(NOT(ISBLANK($A9)),SUM(B$3:B9)-SUM(C$3:C9),"")</f>
+        <v>33.849999999999909</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" s="18">
+        <f>IF(NOT(ISBLANK($A9)),SUM(E$3:E9)-SUM(F$3:F9),"")</f>
+        <v>-56.160000000000011</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="18">
+        <f>IF(NOT(ISBLANK($A9)),SUM(H$3:H9)-SUM(I$3:I9),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>42989</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="14">
+        <v>20</v>
+      </c>
+      <c r="D10" s="18">
+        <f>IF(NOT(ISBLANK($A10)),SUM(B$3:B10)-SUM(C$3:C10),"")</f>
+        <v>13.849999999999909</v>
+      </c>
+      <c r="E10" s="7">
+        <v>20</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="18">
+        <f>IF(NOT(ISBLANK($A10)),SUM(E$3:E10)-SUM(F$3:F10),"")</f>
+        <v>-36.160000000000011</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="18">
+        <f>IF(NOT(ISBLANK($A10)),SUM(H$3:H10)-SUM(I$3:I10),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>42995</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="14">
+        <v>128.26</v>
+      </c>
+      <c r="D11" s="18">
+        <f>IF(NOT(ISBLANK($A11)),SUM(B$3:B11)-SUM(C$3:C11),"")</f>
+        <v>-114.40999999999985</v>
+      </c>
+      <c r="E11" s="7">
+        <v>128.26</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="18">
+        <f>IF(NOT(ISBLANK($A11)),SUM(E$3:E11)-SUM(F$3:F11),"")</f>
+        <v>92.099999999999966</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="18">
+        <f>IF(NOT(ISBLANK($A11)),SUM(H$3:H11)-SUM(I$3:I11),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>42996</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="18">
+        <f>IF(NOT(ISBLANK($A12)),SUM(B$3:B12)-SUM(C$3:C12),"")</f>
+        <v>-114.40999999999985</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="14">
+        <v>92.1</v>
+      </c>
+      <c r="G12" s="18">
+        <f>IF(NOT(ISBLANK($A12)),SUM(E$3:E12)-SUM(F$3:F12),"")</f>
+        <v>-2.8421709430404007E-14</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="18">
+        <f>IF(NOT(ISBLANK($A12)),SUM(H$3:H12)-SUM(I$3:I12),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>42996</v>
+      </c>
+      <c r="B13" s="7">
+        <v>950</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="18">
+        <f>IF(NOT(ISBLANK($A13)),SUM(B$3:B13)-SUM(C$3:C13),"")</f>
+        <v>835.59000000000015</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="18">
+        <f>IF(NOT(ISBLANK($A13)),SUM(E$3:E13)-SUM(F$3:F13),"")</f>
+        <v>-2.8421709430404007E-14</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="18">
+        <f>IF(NOT(ISBLANK($A13)),SUM(H$3:H13)-SUM(I$3:I13),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A14)),SUM(B$3:B14)-SUM(C$3:C14),"")</f>
+        <v/>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A14)),SUM(E$3:E14)-SUM(F$3:F14),"")</f>
+        <v/>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A14)),SUM(H$3:H14)-SUM(I$3:I14),"")</f>
+        <v/>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A15)),SUM(B$3:B15)-SUM(C$3:C15),"")</f>
+        <v/>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A15)),SUM(E$3:E15)-SUM(F$3:F15),"")</f>
+        <v/>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A15)),SUM(H$3:H15)-SUM(I$3:I15),"")</f>
+        <v/>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A16)),SUM(B$3:B16)-SUM(C$3:C16),"")</f>
+        <v/>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A16)),SUM(E$3:E16)-SUM(F$3:F16),"")</f>
+        <v/>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A16)),SUM(H$3:H16)-SUM(I$3:I16),"")</f>
+        <v/>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A17)),SUM(B$3:B17)-SUM(C$3:C17),"")</f>
+        <v/>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A17)),SUM(E$3:E17)-SUM(F$3:F17),"")</f>
+        <v/>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="18" t="str">
+        <f>IF(NOT(ISBLANK($A17)),SUM(H$3:H17)-SUM(I$3:I17),"")</f>
+        <v/>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="40"/>
+    <col min="5" max="5" width="12.140625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="9" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50" style="40" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="40" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" style="40" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="D1" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="97"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="96">
+        <v>2500</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="74"/>
+      <c r="E2" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="72">
+        <v>43160</v>
+      </c>
+      <c r="K2" s="71">
+        <v>43163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="96">
+        <v>830</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="68"/>
+      <c r="H3" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="67">
+        <f>J2-1</f>
+        <v>43159</v>
+      </c>
+      <c r="J3" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="65">
+        <f>K2+1</f>
+        <v>43164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="96">
+        <v>750</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="62"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="96">
+        <v>4782.16</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="72">
+        <v>43267</v>
+      </c>
+      <c r="K5" s="71">
+        <v>43268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="96">
+        <v>4210.3999999999996</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="70"/>
+      <c r="E6" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="68"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="67">
+        <f>J5-IF(L6,1,0)</f>
+        <v>43266</v>
+      </c>
+      <c r="J6" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="65">
+        <f>K5</f>
+        <v>43268</v>
+      </c>
+      <c r="L6" s="107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="78">
+        <v>2500</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="64"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="59"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="86">
+        <f>2*F48</f>
+        <v>3800</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="74"/>
+      <c r="E8" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="72">
+        <v>43279</v>
+      </c>
+      <c r="K8" s="71">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="86">
+        <f>F18+F20</f>
+        <v>1722</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="70"/>
+      <c r="E9" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="68"/>
+      <c r="H9" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="67">
+        <f>J8-1</f>
+        <v>43278</v>
+      </c>
+      <c r="J9" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="65">
+        <f>K8+1</f>
+        <v>43283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="86">
+        <f>F42*(F43+F41*F44)+F45+F41*F46</f>
+        <v>2800</v>
+      </c>
+      <c r="B10" s="50" t="str">
+        <f>"Nationals Winnipeg, "&amp;$F$41&amp;" days"</f>
+        <v>Nationals Winnipeg, 8 days</v>
+      </c>
+      <c r="D10" s="64"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="59"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="86">
+        <f>IF(G23,2*F33+F26*F27*F34+F35+F36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="50" t="str">
+        <f>"Easterns Windsor, "&amp;$F$26&amp;" days (Flying)"</f>
+        <v>Easterns Windsor, 6 days (Flying)</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="51"/>
+      <c r="K11" s="92"/>
+    </row>
+    <row r="12" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="85">
+        <f>SUM(A2:A11)</f>
+        <v>23894.559999999998</v>
+      </c>
+      <c r="B12" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="79">
+        <f>1000*80/1000*1.3</f>
+        <v>104</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="92"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="53"/>
+      <c r="E13" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="78">
+        <v>40</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="95"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="92"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="53"/>
+      <c r="E14" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="78">
+        <v>150</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="50"/>
+    </row>
+    <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="97"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="51">
+        <f>(K3-I3)+(K6-I6)+(K9-I9)</f>
+        <v>12</v>
+      </c>
+      <c r="G15" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="50"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="88">
+        <f>A2</f>
+        <v>2500</v>
+      </c>
+      <c r="B16" s="50" t="str">
+        <f>B2</f>
+        <v>meet fees</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="E16" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="90">
+        <v>2</v>
+      </c>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="50"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="88">
+        <f t="shared" ref="A17:B18" si="0">A3</f>
+        <v>830</v>
+      </c>
+      <c r="B17" s="50" t="str">
+        <f t="shared" si="0"/>
+        <v>Belleville</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="50"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="88">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="B18" s="50" t="str">
+        <f t="shared" si="0"/>
+        <v>Point Claire</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="89">
+        <f>F15*F16</f>
+        <v>24</v>
+      </c>
+      <c r="F18" s="87">
+        <f>E18*F13</f>
+        <v>960</v>
+      </c>
+      <c r="G18" s="51" t="str">
+        <f>(K3-I3)+(K9-I9)&amp;" days of Championships, "&amp;K6-I6&amp;" days of Festival"</f>
+        <v>10 days of Championships, 2 days of Festival</v>
+      </c>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="50"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="88">
+        <f>A5</f>
+        <v>4782.16</v>
+      </c>
+      <c r="B19" s="50" t="str">
+        <f>B5</f>
+        <v>William</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="50"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="88">
+        <f>A6</f>
+        <v>4210.3999999999996</v>
+      </c>
+      <c r="B20" s="50" t="str">
+        <f>B6</f>
+        <v>Olivier</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="E20" s="51">
+        <v>3</v>
+      </c>
+      <c r="F20" s="87">
+        <f>E20*(F14+F12)</f>
+        <v>762</v>
+      </c>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="50"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="88">
+        <f>A7</f>
+        <v>2500</v>
+      </c>
+      <c r="B21" s="50" t="str">
+        <f>B7</f>
+        <v>Olivier Skiing</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="41"/>
+    </row>
+    <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A22" s="88">
+        <f>A8</f>
+        <v>3800</v>
+      </c>
+      <c r="B22" s="50" t="str">
+        <f>B8</f>
+        <v>Training Camp</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="76"/>
+      <c r="J22" s="83">
+        <v>43202</v>
+      </c>
+      <c r="K22" s="82">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="88">
+        <f>A9</f>
+        <v>1722</v>
+      </c>
+      <c r="B23" s="50" t="str">
+        <f>B9</f>
+        <v xml:space="preserve">Toronto Meets </v>
+      </c>
+      <c r="D23" s="104" t="str">
+        <f>IF(G23,"","NOT ")&amp;"ATTENDING"</f>
+        <v>NOT ATTENDING</v>
+      </c>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="101"/>
+      <c r="I23" s="101"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="103"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="88">
+        <f>A10</f>
+        <v>2800</v>
+      </c>
+      <c r="B24" s="50" t="str">
+        <f>B10</f>
+        <v>Nationals Winnipeg, 8 days</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="68"/>
+      <c r="H24" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="67">
+        <f>J22-2</f>
+        <v>43200</v>
+      </c>
+      <c r="J24" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="65">
+        <f>K22+1</f>
+        <v>43206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="86">
+        <f>IF(G23,F28+F26*F27*F30+F31+F29,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B25" s="50" t="str">
+        <f>"Easterns Windsor, "&amp;$F$26&amp;" days (Driving 10 hours)"</f>
+        <v>Easterns Windsor, 6 days (Driving 10 hours)</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="68"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="65"/>
+    </row>
+    <row r="26" spans="1:11" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="85">
+        <f>SUM(A16:A25)</f>
+        <v>23894.559999999998</v>
+      </c>
+      <c r="B26" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="58">
+        <f>K24-I24</f>
+        <v>6</v>
+      </c>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="50"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="98"/>
+      <c r="B27" s="99"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="57">
+        <v>2</v>
+      </c>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="50"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="79">
+        <f>1800*80/1000*1.3</f>
+        <v>187.20000000000002</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="50"/>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="53"/>
+      <c r="E29" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="79">
+        <v>120</v>
+      </c>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="50"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="53"/>
+      <c r="E30" s="51" t="str">
+        <f>E13</f>
+        <v>Food</v>
+      </c>
+      <c r="F30" s="78">
+        <f>F13</f>
+        <v>40</v>
+      </c>
+      <c r="G30" s="79" t="str">
+        <f>G13</f>
+        <v>Per Day/Per person</v>
+      </c>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="50"/>
+    </row>
+    <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A31" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="97"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="51" t="str">
+        <f>E14</f>
+        <v>Grocery</v>
+      </c>
+      <c r="F31" s="78">
+        <f>F14</f>
+        <v>150</v>
+      </c>
+      <c r="G31" s="79" t="str">
+        <f>G14</f>
+        <v>Per Trip</v>
+      </c>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="50"/>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="110">
+        <f>F41+IF(G23,F26,0)+F15</f>
+        <v>20</v>
+      </c>
+      <c r="B32" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="53"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="50"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="80">
+        <v>25000</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="78">
+        <v>450</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="56">
+        <f>I24</f>
+        <v>43200</v>
+      </c>
+      <c r="J33" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="54">
+        <f>K24</f>
+        <v>43206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="109">
+        <f>A33*A32</f>
+        <v>500000</v>
+      </c>
+      <c r="B34" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="53"/>
+      <c r="E34" s="51" t="str">
+        <f>E30</f>
+        <v>Food</v>
+      </c>
+      <c r="F34" s="78">
+        <v>70</v>
+      </c>
+      <c r="G34" s="51" t="str">
+        <f>G30</f>
+        <v>Per Day/Per person</v>
+      </c>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="50"/>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="108">
+        <v>150</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="53"/>
+      <c r="E35" s="51" t="str">
+        <f>E31</f>
+        <v>Grocery</v>
+      </c>
+      <c r="F35" s="78">
+        <v>20</v>
+      </c>
+      <c r="G35" s="51" t="str">
+        <f>G31</f>
+        <v>Per Trip</v>
+      </c>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="50"/>
+    </row>
+    <row r="36" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="85">
+        <f>A32*A35</f>
+        <v>3000</v>
+      </c>
+      <c r="B36" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="44"/>
+      <c r="E36" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="77">
+        <v>80</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="41"/>
+    </row>
+    <row r="37" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="D37" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="I37" s="76"/>
+      <c r="K37" s="75"/>
+    </row>
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="74"/>
+      <c r="E38" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="72">
+        <v>43306</v>
+      </c>
+      <c r="K38" s="71">
+        <v>43311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D39" s="70"/>
+      <c r="E39" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="68"/>
+      <c r="H39" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="67">
+        <f>J38-2</f>
+        <v>43304</v>
+      </c>
+      <c r="J39" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="K39" s="65">
+        <f>K38+1</f>
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="97"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="62"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="59"/>
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="111">
+        <f>'Swim Budget'!A12</f>
+        <v>23894.559999999998</v>
+      </c>
+      <c r="B41" s="112" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="53"/>
+      <c r="E41" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="58">
+        <f>K39-I39</f>
+        <v>8</v>
+      </c>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="50"/>
+    </row>
+    <row r="42" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="113">
+        <v>3950</v>
+      </c>
+      <c r="B42" s="112" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="53"/>
+      <c r="E42" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="57">
+        <v>2</v>
+      </c>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="50"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="117">
+        <v>21</v>
+      </c>
+      <c r="B43" s="116" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="53"/>
+      <c r="E43" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="52">
+        <v>750</v>
+      </c>
+      <c r="G43" s="51" t="str">
+        <f>G33</f>
+        <v>Per Person</v>
+      </c>
+      <c r="H43" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43" s="56">
+        <f>I39</f>
+        <v>43304</v>
+      </c>
+      <c r="J43" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="54">
+        <f>K39</f>
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="121"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="51" t="str">
+        <f>E34</f>
+        <v>Food</v>
+      </c>
+      <c r="F44" s="52">
+        <f>F34</f>
+        <v>70</v>
+      </c>
+      <c r="G44" s="51" t="str">
+        <f>G34</f>
+        <v>Per Day/Per person</v>
+      </c>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="50"/>
+    </row>
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="114">
+        <f>ROUNDUP(C45,-1)</f>
+        <v>950</v>
+      </c>
+      <c r="B45" s="112" t="str">
+        <f>"Rest of this year "&amp;TEXT(C45,"($###.00)")</f>
+        <v>Rest of this year ($949.74)</v>
+      </c>
+      <c r="C45" s="107">
+        <f>(annual_budget-already_paid)/installments_remain</f>
+        <v>949.74095238095231</v>
+      </c>
+      <c r="D45" s="53"/>
+      <c r="E45" s="51" t="str">
+        <f>E35</f>
+        <v>Grocery</v>
+      </c>
+      <c r="F45" s="52">
+        <f>F35</f>
+        <v>20</v>
+      </c>
+      <c r="G45" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="50"/>
+    </row>
+    <row r="46" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="114">
+        <f t="shared" ref="A46:A47" si="1">ROUNDUP(C46,-1)</f>
+        <v>890</v>
+      </c>
+      <c r="B46" s="112" t="str">
+        <f>"Ammortize next year "&amp;TEXT(C46,"($###.00)")</f>
+        <v>Ammortize next year ($889.76)</v>
+      </c>
+      <c r="C46" s="107">
+        <f>((annual_budget-US_training_camp)*2-already_paid)/(installments_remain+24)</f>
+        <v>889.75822222222212</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="42" t="str">
+        <f>E36</f>
+        <v>Cabs</v>
+      </c>
+      <c r="F46" s="49">
+        <v>20</v>
+      </c>
+      <c r="G46" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="41"/>
+    </row>
+    <row r="47" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="115">
+        <f t="shared" si="1"/>
+        <v>840</v>
+      </c>
+      <c r="B47" s="116" t="str">
+        <f>"Next Year Alone "&amp;TEXT(C47,"($###.00)")</f>
+        <v>Next Year Alone ($837.27)</v>
+      </c>
+      <c r="C47" s="107">
+        <f>(annual_budget-2*US_training_camp)/24</f>
+        <v>837.2733333333332</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="45"/>
+    </row>
+    <row r="48" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="118" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="119"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="43">
+        <v>1900</v>
+      </c>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="41"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="114">
+        <f>ROUNDUP(C49,-1)</f>
+        <v>1100</v>
+      </c>
+      <c r="B49" s="112" t="str">
+        <f>"Rest of this year "&amp;TEXT(C49,"($###.00)")</f>
+        <v>Rest of this year ($1092.60)</v>
+      </c>
+      <c r="C49" s="107">
+        <f>(annual_budget+hotel_cost-already_paid)/installments_remain</f>
+        <v>1092.5980952380951</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="114">
+        <f t="shared" ref="A50:A51" si="2">ROUNDUP(C50,-1)</f>
+        <v>1030</v>
+      </c>
+      <c r="B50" s="112" t="str">
+        <f>"Ammortize next year "&amp;TEXT(C50,"($###.00)")</f>
+        <v>Ammortize next year ($1023.09)</v>
+      </c>
+      <c r="C50" s="107">
+        <f>((annual_budget+hotel_cost-US_training_camp)*2-already_paid)/(installments_remain+24)</f>
+        <v>1023.0915555555555</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="115">
+        <f t="shared" si="2"/>
+        <v>970</v>
+      </c>
+      <c r="B51" s="116" t="str">
+        <f>"Next Year Alone "&amp;TEXT(C51,"($###.00)")</f>
+        <v>Next Year Alone ($962.27)</v>
+      </c>
+      <c r="C51" s="107">
+        <f>(annual_budget+hotel_cost-2*US_training_camp)/24</f>
+        <v>962.2733333333332</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="48">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F25:G25"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D22:K36">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>NOT($G$23)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="48" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4097" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Festival_Early_Checkin">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="122">
+        <v>2123.0300000000002</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="122"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="122">
+        <v>-400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="122">
+        <v>-450</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="122">
+        <v>-75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="122">
+        <v>-100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="122">
+        <v>-950</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="122">
+        <v>-50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="122">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="122">
+        <f>SUM(A1:A8)</f>
+        <v>98.0300000000002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated christmas account transfers.
</commit_message>
<xml_diff>
--- a/book-keeping.xlsx
+++ b/book-keeping.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="165">
   <si>
     <t>Date</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>Refund</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Yup.  Transferred twice.</t>
   </si>
 </sst>
 </file>
@@ -1371,22 +1377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="10" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1395,14 +1389,8 @@
     <xf numFmtId="15" fontId="10" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1419,13 +1407,31 @@
     <xf numFmtId="15" fontId="11" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8737,10 +8743,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8755,9 +8761,10 @@
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
@@ -8775,7 +8782,7 @@
         <v>132</v>
       </c>
       <c r="I1" s="111" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="J1" s="111" t="s">
         <v>133</v>
@@ -8786,8 +8793,11 @@
       <c r="L1" s="111" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="111" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="112"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -8812,613 +8822,658 @@
       <c r="J2" s="112"/>
       <c r="K2" s="112"/>
       <c r="L2" s="112"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="M2" s="112"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>42996</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>100</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="18">
+      <c r="C3" s="15"/>
+      <c r="D3" s="19">
         <f>IF(NOT(ISBLANK($A3)),SUM(B$3:B3)-SUM(C$3:C3),"")</f>
         <v>100</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="18">
+      <c r="E3" s="9"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="19">
         <f>IF(NOT(ISBLANK($A3)),SUM(E$3:E3)-SUM(F$3:F3),"")</f>
         <v>0</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="100">
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="101">
         <f>IF(NOT(ISBLANK(A3)),SUMIF($J$3:$J3,$J3,$F$3:$F3)-SUMIF($J$3:$J3,$J3,$E$3:$E3),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>43009</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="18">
+      <c r="B4" s="9"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="19">
         <f>IF(NOT(ISBLANK($A4)),SUM(B$3:B4)-SUM(C$3:C4),"")</f>
         <v>100</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="14">
+      <c r="E4" s="9"/>
+      <c r="F4" s="15">
         <v>14.68</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="19">
         <f>IF(NOT(ISBLANK($A4)),SUM(E$3:E4)-SUM(F$3:F4),"")</f>
         <v>-14.68</v>
       </c>
-      <c r="H4" s="8" t="b">
+      <c r="H4" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="L4" s="100">
+      <c r="L4" s="101">
         <f>IF(NOT(ISBLANK(A4)),SUMIF($J$3:$J4,$J4,$F$3:$F4)-SUMIF($J$3:$J4,$J4,$E$3:$E4),"")</f>
         <v>14.68</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>43009</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="15">
+      <c r="B5" s="7"/>
+      <c r="C5" s="14">
         <v>14.68</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <f>IF(NOT(ISBLANK($A5)),SUM(B$3:B5)-SUM(C$3:C5),"")</f>
         <v>85.32</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>14.68</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="19">
+      <c r="F5" s="14"/>
+      <c r="G5" s="18">
         <f>IF(NOT(ISBLANK($A5)),SUM(E$3:E5)-SUM(F$3:F5),"")</f>
         <v>0</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="101">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="100">
         <f>IF(NOT(ISBLANK(A5)),SUMIF($J$3:$J5,$J5,$F$3:$F5)-SUMIF($J$3:$J5,$J5,$E$3:$E5),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>43010</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>0.03</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="19">
+      <c r="C6" s="14"/>
+      <c r="D6" s="18">
         <f>IF(NOT(ISBLANK($A6)),SUM(B$3:B6)-SUM(C$3:C6),"")</f>
         <v>85.35</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="19">
+      <c r="E6" s="7"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="18">
         <f>IF(NOT(ISBLANK($A6)),SUM(E$3:E6)-SUM(F$3:F6),"")</f>
         <v>0</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="101">
+      <c r="L6" s="100">
         <f>IF(NOT(ISBLANK(A6)),SUMIF($J$3:$J6,$J6,$F$3:$F6)-SUMIF($J$3:$J6,$J6,$E$3:$E6),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>43011</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <v>100</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="18">
+      <c r="C7" s="15"/>
+      <c r="D7" s="19">
         <f>IF(NOT(ISBLANK($A7)),SUM(B$3:B7)-SUM(C$3:C7),"")</f>
         <v>185.35</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="18">
+      <c r="E7" s="9"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="19">
         <f>IF(NOT(ISBLANK($A7)),SUM(E$3:E7)-SUM(F$3:F7),"")</f>
         <v>0</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="100">
+      <c r="L7" s="101">
         <f>IF(NOT(ISBLANK(A7)),SUMIF($J$3:$J7,$J7,$F$3:$F7)-SUMIF($J$3:$J7,$J7,$E$3:$E7),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>43026</v>
-      </c>
-      <c r="B8" s="7">
-        <v>100</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="18">
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>43025</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="15">
+        <v>8.43</v>
+      </c>
+      <c r="D8" s="19">
         <f>IF(NOT(ISBLANK($A8)),SUM(B$3:B8)-SUM(C$3:C8),"")</f>
-        <v>285.34999999999997</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="18">
+        <v>176.92000000000002</v>
+      </c>
+      <c r="E8" s="9">
+        <v>8.43</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="19">
         <f>IF(NOT(ISBLANK($A8)),SUM(E$3:E8)-SUM(F$3:F8),"")</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="100">
+        <v>8.43</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="101">
         <f>IF(NOT(ISBLANK(A8)),SUMIF($J$3:$J8,$J8,$F$3:$F8)-SUMIF($J$3:$J8,$J8,$E$3:$E8),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="M8" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>43026</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="19">
+      <c r="B9" s="7">
+        <v>100</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="18">
         <f>IF(NOT(ISBLANK($A9)),SUM(B$3:B9)-SUM(C$3:C9),"")</f>
-        <v>285.34999999999997</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="15">
+        <v>276.91999999999996</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="18">
+        <f>IF(NOT(ISBLANK($A9)),SUM(E$3:E9)-SUM(F$3:F9),"")</f>
         <v>8.43</v>
       </c>
-      <c r="G9" s="19">
-        <f>IF(NOT(ISBLANK($A9)),SUM(E$3:E9)-SUM(F$3:F9),"")</f>
-        <v>-8.43</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="100">
+        <f>IF(NOT(ISBLANK(A9)),SUMIF($J$3:$J9,$J9,$F$3:$F9)-SUMIF($J$3:$J9,$J9,$E$3:$E9),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>43026</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="18">
+        <f>IF(NOT(ISBLANK($A10)),SUM(B$3:B10)-SUM(C$3:C10),"")</f>
+        <v>276.91999999999996</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="14">
+        <v>8.43</v>
+      </c>
+      <c r="G10" s="18">
+        <f>IF(NOT(ISBLANK($A10)),SUM(E$3:E10)-SUM(F$3:F10),"")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K10" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="L9" s="101">
-        <f>IF(NOT(ISBLANK(A9)),SUMIF($J$3:$J9,$J9,$F$3:$F9)-SUMIF($J$3:$J9,$J9,$E$3:$E9),"")</f>
+      <c r="L10" s="100">
+        <f>IF(NOT(ISBLANK(A10)),SUMIF($J$3:$J10,$J10,$F$3:$F10)-SUMIF($J$3:$J10,$J10,$E$3:$E10),"")</f>
         <v>8.43</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>43028</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="19">
-        <f>IF(NOT(ISBLANK($A10)),SUM(B$3:B10)-SUM(C$3:C10),"")</f>
-        <v>285.34999999999997</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="15">
+      <c r="B11" s="9"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="19">
+        <f>IF(NOT(ISBLANK($A11)),SUM(B$3:B11)-SUM(C$3:C11),"")</f>
+        <v>276.91999999999996</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="15">
         <v>220.72</v>
       </c>
-      <c r="G10" s="19">
-        <f>IF(NOT(ISBLANK($A10)),SUM(E$3:E10)-SUM(F$3:F10),"")</f>
-        <v>-229.14999999999998</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
+      <c r="G11" s="19">
+        <f>IF(NOT(ISBLANK($A11)),SUM(E$3:E11)-SUM(F$3:F11),"")</f>
+        <v>-220.71999999999997</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J11" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L10" s="101">
-        <f>IF(NOT(ISBLANK(A10)),SUMIF($J$3:$J10,$J10,$F$3:$F10)-SUMIF($J$3:$J10,$J10,$E$3:$E10),"")</f>
+      <c r="L11" s="101">
+        <f>IF(NOT(ISBLANK(A11)),SUMIF($J$3:$J11,$J11,$F$3:$F11)-SUMIF($J$3:$J11,$J11,$E$3:$E11),"")</f>
         <v>220.72</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>43028</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="18">
-        <f>IF(NOT(ISBLANK($A11)),SUM(B$3:B11)-SUM(C$3:C11),"")</f>
-        <v>285.34999999999997</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="14">
+      <c r="B12" s="9"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="19">
+        <f>IF(NOT(ISBLANK($A12)),SUM(B$3:B12)-SUM(C$3:C12),"")</f>
+        <v>276.91999999999996</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="15">
         <v>108.41</v>
       </c>
-      <c r="G11" s="18">
-        <f>IF(NOT(ISBLANK($A11)),SUM(E$3:E11)-SUM(F$3:F11),"")</f>
-        <v>-337.56</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
+      <c r="G12" s="19">
+        <f>IF(NOT(ISBLANK($A12)),SUM(E$3:E12)-SUM(F$3:F12),"")</f>
+        <v>-329.13</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J12" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K12" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L11" s="100">
-        <f>IF(NOT(ISBLANK(A11)),SUMIF($J$3:$J11,$J11,$F$3:$F11)-SUMIF($J$3:$J11,$J11,$E$3:$E11),"")</f>
+      <c r="L12" s="101">
+        <f>IF(NOT(ISBLANK(A12)),SUMIF($J$3:$J12,$J12,$F$3:$F12)-SUMIF($J$3:$J12,$J12,$E$3:$E12),"")</f>
         <v>329.13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>43029</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="18">
-        <f>IF(NOT(ISBLANK($A12)),SUM(B$3:B12)-SUM(C$3:C12),"")</f>
-        <v>285.34999999999997</v>
-      </c>
-      <c r="E12" s="7">
-        <v>10.11</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="18">
-        <f>IF(NOT(ISBLANK($A12)),SUM(E$3:E12)-SUM(F$3:F12),"")</f>
-        <v>-327.45</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="L12" s="100">
-        <f>IF(NOT(ISBLANK(A12)),SUMIF($J$3:$J12,$J12,$F$3:$F12)-SUMIF($J$3:$J12,$J12,$E$3:$E12),"")</f>
-        <v>319.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>43031</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="15">
-        <v>220.72</v>
-      </c>
-      <c r="D13" s="19">
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>43028</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="14">
+        <v>8.43</v>
+      </c>
+      <c r="D13" s="18">
         <f>IF(NOT(ISBLANK($A13)),SUM(B$3:B13)-SUM(C$3:C13),"")</f>
-        <v>64.629999999999967</v>
-      </c>
-      <c r="E13" s="9">
-        <v>220.72</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="19">
+        <v>268.48999999999995</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8.43</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="18">
         <f>IF(NOT(ISBLANK($A13)),SUM(E$3:E13)-SUM(F$3:F13),"")</f>
-        <v>-106.73000000000002</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
+        <v>-320.7</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="101">
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="100">
         <f>IF(NOT(ISBLANK(A13)),SUMIF($J$3:$J13,$J13,$F$3:$F13)-SUMIF($J$3:$J13,$J13,$E$3:$E13),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="19" t="str">
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>43029</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="18">
         <f>IF(NOT(ISBLANK($A14)),SUM(B$3:B14)-SUM(C$3:C14),"")</f>
-        <v/>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="19" t="str">
+        <v>268.48999999999995</v>
+      </c>
+      <c r="E14" s="7">
+        <v>10.11</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="18">
         <f>IF(NOT(ISBLANK($A14)),SUM(E$3:E14)-SUM(F$3:F14),"")</f>
-        <v/>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="101" t="str">
+        <v>-310.59000000000003</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L14" s="100">
         <f>IF(NOT(ISBLANK(A14)),SUMIF($J$3:$J14,$J14,$F$3:$F14)-SUMIF($J$3:$J14,$J14,$E$3:$E14),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="18" t="str">
+        <v>319.02</v>
+      </c>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>43031</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="15">
+        <v>220.72</v>
+      </c>
+      <c r="D15" s="19">
         <f>IF(NOT(ISBLANK($A15)),SUM(B$3:B15)-SUM(C$3:C15),"")</f>
-        <v/>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="18" t="str">
+        <v>47.769999999999982</v>
+      </c>
+      <c r="E15" s="9">
+        <v>220.72</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="19">
         <f>IF(NOT(ISBLANK($A15)),SUM(E$3:E15)-SUM(F$3:F15),"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="100" t="str">
+        <v>-89.87</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="101">
         <f>IF(NOT(ISBLANK(A15)),SUMIF($J$3:$J15,$J15,$F$3:$F15)-SUMIF($J$3:$J15,$J15,$E$3:$E15),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="18" t="str">
+        <v>0</v>
+      </c>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="19" t="str">
         <f>IF(NOT(ISBLANK($A16)),SUM(B$3:B16)-SUM(C$3:C16),"")</f>
         <v/>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="18" t="str">
+      <c r="E16" s="9"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="19" t="str">
         <f>IF(NOT(ISBLANK($A16)),SUM(E$3:E16)-SUM(F$3:F16),"")</f>
         <v/>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="100" t="str">
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="101" t="str">
         <f>IF(NOT(ISBLANK(A16)),SUMIF($J$3:$J16,$J16,$F$3:$F16)-SUMIF($J$3:$J16,$J16,$E$3:$E16),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="19" t="str">
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="18" t="str">
         <f>IF(NOT(ISBLANK($A17)),SUM(B$3:B17)-SUM(C$3:C17),"")</f>
         <v/>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="19" t="str">
+      <c r="E17" s="7"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="18" t="str">
         <f>IF(NOT(ISBLANK($A17)),SUM(E$3:E17)-SUM(F$3:F17),"")</f>
         <v/>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="101" t="str">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="100" t="str">
         <f>IF(NOT(ISBLANK(A17)),SUMIF($J$3:$J17,$J17,$F$3:$F17)-SUMIF($J$3:$J17,$J17,$E$3:$E17),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="19" t="str">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="18" t="str">
         <f>IF(NOT(ISBLANK($A18)),SUM(B$3:B18)-SUM(C$3:C18),"")</f>
         <v/>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="19" t="str">
+      <c r="E18" s="7"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="18" t="str">
         <f>IF(NOT(ISBLANK($A18)),SUM(E$3:E18)-SUM(F$3:F18),"")</f>
         <v/>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="101" t="str">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="100" t="str">
         <f>IF(NOT(ISBLANK(A18)),SUMIF($J$3:$J18,$J18,$F$3:$F18)-SUMIF($J$3:$J18,$J18,$E$3:$E18),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="18" t="str">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="19" t="str">
         <f>IF(NOT(ISBLANK($A19)),SUM(B$3:B19)-SUM(C$3:C19),"")</f>
         <v/>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="18" t="str">
+      <c r="E19" s="9"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="19" t="str">
         <f>IF(NOT(ISBLANK($A19)),SUM(E$3:E19)-SUM(F$3:F19),"")</f>
         <v/>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="100" t="str">
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="101" t="str">
         <f>IF(NOT(ISBLANK(A19)),SUMIF($J$3:$J19,$J19,$F$3:$F19)-SUMIF($J$3:$J19,$J19,$E$3:$E19),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="18" t="str">
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="19" t="str">
         <f>IF(NOT(ISBLANK($A20)),SUM(B$3:B20)-SUM(C$3:C20),"")</f>
         <v/>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="18" t="str">
+      <c r="E20" s="9"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="19" t="str">
         <f>IF(NOT(ISBLANK($A20)),SUM(E$3:E20)-SUM(F$3:F20),"")</f>
         <v/>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="100" t="str">
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="101" t="str">
         <f>IF(NOT(ISBLANK(A20)),SUMIF($J$3:$J20,$J20,$F$3:$F20)-SUMIF($J$3:$J20,$J20,$E$3:$E20),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="19" t="str">
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="18" t="str">
         <f>IF(NOT(ISBLANK($A21)),SUM(B$3:B21)-SUM(C$3:C21),"")</f>
         <v/>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="19" t="str">
+      <c r="E21" s="7"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="18" t="str">
         <f>IF(NOT(ISBLANK($A21)),SUM(E$3:E21)-SUM(F$3:F21),"")</f>
         <v/>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="101" t="str">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="100" t="str">
         <f>IF(NOT(ISBLANK(A21)),SUMIF($J$3:$J21,$J21,$F$3:$F21)-SUMIF($J$3:$J21,$J21,$E$3:$E21),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="19" t="str">
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="18" t="str">
         <f>IF(NOT(ISBLANK($A22)),SUM(B$3:B22)-SUM(C$3:C22),"")</f>
         <v/>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="19" t="str">
+      <c r="E22" s="7"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="18" t="str">
         <f>IF(NOT(ISBLANK($A22)),SUM(E$3:E22)-SUM(F$3:F22),"")</f>
         <v/>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="101" t="str">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="100" t="str">
         <f>IF(NOT(ISBLANK(A22)),SUMIF($J$3:$J22,$J22,$F$3:$F22)-SUMIF($J$3:$J22,$J22,$E$3:$E22),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="18" t="str">
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="19" t="str">
         <f>IF(NOT(ISBLANK($A23)),SUM(B$3:B23)-SUM(C$3:C23),"")</f>
         <v/>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="18" t="str">
+      <c r="E23" s="9"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="19" t="str">
         <f>IF(NOT(ISBLANK($A23)),SUM(E$3:E23)-SUM(F$3:F23),"")</f>
         <v/>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="100" t="str">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="101" t="str">
         <f>IF(NOT(ISBLANK(A23)),SUMIF($J$3:$J23,$J23,$F$3:$F23)-SUMIF($J$3:$J23,$J23,$E$3:$E23),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18" t="str">
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="19" t="str">
         <f>IF(NOT(ISBLANK($A24)),SUM(B$3:B24)-SUM(C$3:C24),"")</f>
         <v/>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="18" t="str">
+      <c r="E24" s="9"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="19" t="str">
         <f>IF(NOT(ISBLANK($A24)),SUM(E$3:E24)-SUM(F$3:F24),"")</f>
         <v/>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="100" t="str">
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="101" t="str">
         <f>IF(NOT(ISBLANK(A24)),SUMIF($J$3:$J24,$J24,$F$3:$F24)-SUMIF($J$3:$J24,$J24,$E$3:$E24),"")</f>
         <v/>
       </c>
+      <c r="M24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <sortState ref="A3:M16">
+    <sortCondition ref="A3:A16"/>
+  </sortState>
+  <mergeCells count="9">
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
@@ -9600,20 +9655,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="D1" s="118" t="s">
+      <c r="B1" s="132"/>
+      <c r="D1" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="120"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="132"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="77">
@@ -9623,13 +9678,13 @@
         <v>109</v>
       </c>
       <c r="D2" s="56"/>
-      <c r="E2" s="129" t="s">
+      <c r="E2" s="123" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="55">
         <v>43160</v>
       </c>
@@ -9645,24 +9700,24 @@
         <v>111</v>
       </c>
       <c r="D3" s="53"/>
-      <c r="E3" s="127" t="s">
+      <c r="E3" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="121" t="s">
+      <c r="F3" s="128" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="121"/>
-      <c r="H3" s="130" t="s">
+      <c r="G3" s="128"/>
+      <c r="H3" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="132">
+      <c r="I3" s="126">
         <f>J2-1</f>
         <v>43159</v>
       </c>
-      <c r="J3" s="130" t="s">
+      <c r="J3" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="124">
+      <c r="K3" s="120">
         <f>K2+1</f>
         <v>43164</v>
       </c>
@@ -9675,15 +9730,15 @@
         <v>112</v>
       </c>
       <c r="D4" s="52"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="134" t="s">
+      <c r="E4" s="130"/>
+      <c r="F4" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="134"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="125"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="121"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="77">
@@ -9693,13 +9748,13 @@
         <v>107</v>
       </c>
       <c r="D5" s="56"/>
-      <c r="E5" s="129" t="s">
+      <c r="E5" s="123" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="129"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="55">
         <v>43267</v>
       </c>
@@ -9715,22 +9770,22 @@
         <v>106</v>
       </c>
       <c r="D6" s="53"/>
-      <c r="E6" s="127" t="s">
+      <c r="E6" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="121" t="s">
+      <c r="F6" s="128" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="121"/>
+      <c r="G6" s="128"/>
       <c r="H6" s="85"/>
-      <c r="I6" s="132">
+      <c r="I6" s="126">
         <f>J5-IF(L6,1,0)</f>
         <v>43266</v>
       </c>
-      <c r="J6" s="130" t="s">
+      <c r="J6" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="124">
+      <c r="K6" s="120">
         <f>K5</f>
         <v>43268</v>
       </c>
@@ -9746,15 +9801,15 @@
         <v>105</v>
       </c>
       <c r="D7" s="52"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="134" t="s">
+      <c r="E7" s="130"/>
+      <c r="F7" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="134"/>
+      <c r="G7" s="122"/>
       <c r="H7" s="86"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="125"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="121"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="67">
@@ -9765,13 +9820,13 @@
         <v>57</v>
       </c>
       <c r="D8" s="56"/>
-      <c r="E8" s="129" t="s">
+      <c r="E8" s="123" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
       <c r="J8" s="55">
         <v>43279</v>
       </c>
@@ -9788,24 +9843,24 @@
         <v>102</v>
       </c>
       <c r="D9" s="53"/>
-      <c r="E9" s="127" t="s">
+      <c r="E9" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="121" t="s">
+      <c r="F9" s="128" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="121"/>
-      <c r="H9" s="130" t="s">
+      <c r="G9" s="128"/>
+      <c r="H9" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="132">
+      <c r="I9" s="126">
         <f>J8-1</f>
         <v>43278</v>
       </c>
-      <c r="J9" s="130" t="s">
+      <c r="J9" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="124">
+      <c r="K9" s="120">
         <f>K8+1</f>
         <v>43283</v>
       </c>
@@ -9820,15 +9875,15 @@
         <v>Nationals Winnipeg, 8 days</v>
       </c>
       <c r="D10" s="52"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="134" t="s">
+      <c r="E10" s="130"/>
+      <c r="F10" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="134"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="125"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="121"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67">
@@ -9899,10 +9954,10 @@
       <c r="K14" s="43"/>
     </row>
     <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="120"/>
+      <c r="B15" s="132"/>
       <c r="D15" s="46"/>
       <c r="E15" s="44" t="s">
         <v>63</v>
@@ -10058,12 +10113,12 @@
         <f t="shared" si="1"/>
         <v>Training Camp</v>
       </c>
-      <c r="D22" s="118" t="s">
+      <c r="D22" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="119"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
       <c r="H22" s="58" t="s">
         <v>87</v>
       </c>
@@ -10108,24 +10163,24 @@
         <v>Nationals Winnipeg, 8 days</v>
       </c>
       <c r="D24" s="46"/>
-      <c r="E24" s="126" t="s">
+      <c r="E24" s="133" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="121" t="s">
+      <c r="F24" s="128" t="s">
         <v>85</v>
       </c>
-      <c r="G24" s="121"/>
-      <c r="H24" s="130" t="s">
+      <c r="G24" s="128"/>
+      <c r="H24" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="132">
+      <c r="I24" s="126">
         <f>J22-2</f>
         <v>43200</v>
       </c>
-      <c r="J24" s="130" t="s">
+      <c r="J24" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="124">
+      <c r="K24" s="120">
         <f>K22+1</f>
         <v>43206</v>
       </c>
@@ -10140,15 +10195,15 @@
         <v>Easterns Windsor, 6 days (Driving 10 hours)</v>
       </c>
       <c r="D25" s="46"/>
-      <c r="E25" s="126"/>
-      <c r="F25" s="121" t="s">
+      <c r="E25" s="133"/>
+      <c r="F25" s="128" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="121"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="132"/>
-      <c r="J25" s="130"/>
-      <c r="K25" s="124"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="124"/>
+      <c r="K25" s="120"/>
     </row>
     <row r="26" spans="1:11" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="66">
@@ -10241,10 +10296,10 @@
       <c r="K30" s="43"/>
     </row>
     <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="118" t="s">
+      <c r="A31" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="120"/>
+      <c r="B31" s="132"/>
       <c r="D31" s="46"/>
       <c r="E31" s="44" t="str">
         <f t="shared" si="2"/>
@@ -10393,12 +10448,12 @@
       <c r="B37" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="118" t="s">
+      <c r="D37" s="131" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="119"/>
+      <c r="E37" s="134"/>
+      <c r="F37" s="134"/>
+      <c r="G37" s="134"/>
       <c r="I37" s="58"/>
       <c r="K37" s="57"/>
     </row>
@@ -10411,13 +10466,13 @@
         <v>117</v>
       </c>
       <c r="D38" s="56"/>
-      <c r="E38" s="129" t="s">
+      <c r="E38" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="129"/>
-      <c r="G38" s="129"/>
-      <c r="H38" s="129"/>
-      <c r="I38" s="129"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="123"/>
       <c r="J38" s="55">
         <v>43306</v>
       </c>
@@ -10427,39 +10482,39 @@
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D39" s="53"/>
-      <c r="E39" s="127" t="s">
+      <c r="E39" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="121" t="s">
+      <c r="F39" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="121"/>
-      <c r="H39" s="130" t="s">
+      <c r="G39" s="128"/>
+      <c r="H39" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="I39" s="132">
+      <c r="I39" s="126">
         <f>J38-2</f>
         <v>43304</v>
       </c>
-      <c r="J39" s="130" t="s">
+      <c r="J39" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="K39" s="124">
+      <c r="K39" s="120">
         <f>K38+1</f>
         <v>43312</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D40" s="52"/>
-      <c r="E40" s="128"/>
-      <c r="F40" s="134" t="s">
+      <c r="E40" s="130"/>
+      <c r="F40" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="134"/>
-      <c r="H40" s="131"/>
-      <c r="I40" s="133"/>
-      <c r="J40" s="131"/>
-      <c r="K40" s="125"/>
+      <c r="G40" s="122"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="127"/>
+      <c r="J40" s="125"/>
+      <c r="K40" s="121"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="46"/>
@@ -10477,10 +10532,10 @@
       <c r="K41" s="43"/>
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="118" t="s">
+      <c r="A42" s="131" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="120"/>
+      <c r="B42" s="132"/>
       <c r="D42" s="46"/>
       <c r="E42" s="44" t="s">
         <v>62</v>
@@ -10582,10 +10637,10 @@
       <c r="K45" s="43"/>
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="122" t="s">
+      <c r="A46" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="123"/>
+      <c r="B46" s="136"/>
       <c r="C46" s="87">
         <f>((annual_budget-US_training_camp)*2-already_paid)/(installments_remain+24)</f>
         <v>889.75822222222212</v>
@@ -10619,12 +10674,12 @@
         <f>(annual_budget-2*US_training_camp)/24</f>
         <v>837.2733333333332</v>
       </c>
-      <c r="D47" s="118" t="s">
+      <c r="D47" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="119"/>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="134"/>
+      <c r="G47" s="134"/>
       <c r="H47" s="41"/>
       <c r="I47" s="41"/>
       <c r="J47" s="41"/>
@@ -10667,10 +10722,10 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="135" t="s">
+      <c r="A50" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="B50" s="136"/>
+      <c r="B50" s="119"/>
       <c r="C50" s="87">
         <f>((annual_budget+hotel_cost-US_training_camp)*2-already_paid)/(installments_remain+24)</f>
         <v>1029.7582222222222</v>
@@ -10713,6 +10768,38 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="48">
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="F7:G7"/>
@@ -10729,38 +10816,6 @@
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="D22:K36">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>